<commit_message>
change n6 gateway IP
</commit_message>
<xml_diff>
--- a/Chart-customization-checklist.xlsx
+++ b/Chart-customization-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bee369f06cde55e4/_A lot of training/4G ^0 5G/towards5gs-helm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{B5470EC1-0D83-4FA3-B351-3F533031221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F58A649A-8E21-4455-9321-AEAE1DE4BA24}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{B5470EC1-0D83-4FA3-B351-3F533031221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{147A97CE-3F84-4CC6-B477-64F937AB7BF7}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="17880" windowWidth="19440" windowHeight="11520" xr2:uid="{A89B8CCF-D1AF-4C49-B6D5-8DC965BE883F}"/>
+    <workbookView minimized="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9960" xr2:uid="{A89B8CCF-D1AF-4C49-B6D5-8DC965BE883F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>global.n2network.masterIf</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>10.0.2.15</t>
+  </si>
+  <si>
+    <t>10.0.2.2</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,12 +615,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1"/>
     </row>

</xml_diff>

<commit_message>
Change n6 IP address
</commit_message>
<xml_diff>
--- a/Chart-customization-checklist.xlsx
+++ b/Chart-customization-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bee369f06cde55e4/_A lot of training/4G ^0 5G/towards5gs-helm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{B5470EC1-0D83-4FA3-B351-3F533031221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92EF2D62-B820-4A20-89C6-F7B53059CBC5}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{B5470EC1-0D83-4FA3-B351-3F533031221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3042B21-CDAB-4A50-940F-D60621146ED1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A89B8CCF-D1AF-4C49-B6D5-8DC965BE883F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>global.n2network.masterIf</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Interface</t>
+  </si>
+  <si>
+    <t>10.0.2.0</t>
   </si>
 </sst>
 </file>
@@ -204,9 +207,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -244,7 +247,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -350,7 +353,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -492,7 +495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -503,7 +506,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:F13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,12 +617,12 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -645,7 +648,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1"/>
     </row>

</xml_diff>